<commit_message>
filename validataion removed, template_code in lot upload removed
</commit_message>
<xml_diff>
--- a/upload_templates/lots_template.xlsx
+++ b/upload_templates/lots_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\COA_pdf_generator\upload_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FC7EADA-0DB2-485B-85D2-CD965214B19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E9C4A3-7BDB-46A1-99C9-44C8E969EED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{55680B4E-E23E-4AA8-9EB1-85CC769C8677}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{55680B4E-E23E-4AA8-9EB1-85CC769C8677}"/>
   </bookViews>
   <sheets>
     <sheet name="lots_template" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>templateCode</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>lotNumber</t>
   </si>
@@ -881,13 +878,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5164F3CC-541E-442B-B636-528B1A46C198}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -906,9 +905,6 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>